<commit_message>
PaintPanel Code aufgeräumt. Weitere Sttistik Folie hinzugefügt
</commit_message>
<xml_diff>
--- a/Ants/src/doku/Statistik.xlsx
+++ b/Ants/src/doku/Statistik.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>StoryCard</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>Risiko</t>
+  </si>
+  <si>
+    <t>Story Card</t>
+  </si>
+  <si>
+    <t>Verhätnis D/SP</t>
   </si>
 </sst>
 </file>
@@ -131,6 +137,21 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE"/>
+              <a:t>Dauer und Story Points</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
     </c:title>
@@ -138,18 +159,76 @@
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
-        <c:grouping val="standard"/>
+        <c:grouping val="stacked"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Story Points</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$C$2:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>70</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
               <c:f>Tabelle1!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Story Points pro Stunden</c:v>
+                  <c:v>Dauer [min]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -157,73 +236,41 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Tabelle1!$A$2:$A$11</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>Graphische Anzeige des TSP</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Graphische Anzeige der Lösung</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Eigenes Problem erzeugen</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>TSP-Laden</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Parameterkonfiguration</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Berechnung starten</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Anzahl der Iterationen und Ameisen</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Problem Speichern</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Optimale Tour</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Punkte verschiebbar</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Tabelle1!$D$2:$D$11</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>41.25</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41.53846153846154</c:v>
+                  <c:v>130</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>33.333333333333336</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>12</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>15</c:v>
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>120</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -240,11 +287,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="70940672"/>
-        <c:axId val="189834368"/>
+        <c:axId val="137738240"/>
+        <c:axId val="152464768"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="70940672"/>
+        <c:axId val="137738240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -254,7 +301,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="189834368"/>
+        <c:crossAx val="152464768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -262,27 +309,29 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="189834368"/>
+        <c:axId val="152464768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="45"/>
-          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70940672"/>
+        <c:crossAx val="137738240"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-        <c:majorUnit val="10"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
+    <c:dispBlanksAs val="zero"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
@@ -318,7 +367,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="de-DE"/>
-              <a:t>Wert, Risiko, SPpH</a:t>
+              <a:t>Wert und Risiko</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -328,20 +377,30 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.5777938285007739E-2"/>
+          <c:y val="0.20869240303295422"/>
+          <c:w val="0.78103637206057952"/>
+          <c:h val="0.6753277194517352"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$D$1</c:f>
+              <c:f>Tabelle1!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Story Points pro Stunden</c:v>
+                  <c:v>Wert</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -349,73 +408,41 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Tabelle1!$A$2:$A$11</c:f>
-              <c:strCache>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$F$2:$F$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>Graphische Anzeige des TSP</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Graphische Anzeige der Lösung</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Eigenes Problem erzeugen</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>TSP-Laden</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Parameterkonfiguration</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Berechnung starten</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Anzahl der Iterationen und Ameisen</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Problem Speichern</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Optimale Tour</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Punkte verschiebbar</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Tabelle1!$D$2:$D$11</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>41.25</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>41.53846153846154</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>33.333333333333336</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>10</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>15</c:v>
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -423,15 +450,15 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="3"/>
+          <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$E$1</c:f>
+              <c:f>Tabelle1!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Wert</c:v>
+                  <c:v>Risiko</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -439,143 +466,9 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Tabelle1!$A$2:$A$11</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>Graphische Anzeige des TSP</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Graphische Anzeige der Lösung</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Eigenes Problem erzeugen</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>TSP-Laden</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Parameterkonfiguration</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Berechnung starten</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Anzahl der Iterationen und Ameisen</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Problem Speichern</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Optimale Tour</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Punkte verschiebbar</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$E$2:$E$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Tabelle1!$F$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Risiko</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Tabelle1!$A$2:$A$11</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>Graphische Anzeige des TSP</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Graphische Anzeige der Lösung</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Eigenes Problem erzeugen</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>TSP-Laden</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Parameterkonfiguration</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Berechnung starten</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Anzahl der Iterationen und Ameisen</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Problem Speichern</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Optimale Tour</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Punkte verschiebbar</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Tabelle1!$F$2:$F$11</c:f>
+              <c:f>Tabelle1!$G$2:$G$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -624,11 +517,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="124888576"/>
-        <c:axId val="165093376"/>
+        <c:axId val="74276864"/>
+        <c:axId val="151878400"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="124888576"/>
+        <c:axId val="74276864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -638,7 +531,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="165093376"/>
+        <c:crossAx val="151878400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -646,23 +539,221 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="165093376"/>
+        <c:axId val="151878400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="45"/>
-          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124888576"/>
+        <c:crossAx val="74276864"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-        <c:majorUnit val="10"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Story Points pro Stunden</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$E$2:$E$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>41.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41.53846153846154</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>33.333333333333336</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>35</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Story Points</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$C$2:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>70</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="116036608"/>
+        <c:axId val="170808384"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="116036608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="170808384"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="170808384"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="116036608"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -687,19 +778,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>119062</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>423862</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>166687</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Diagramm 7"/>
+        <xdr:cNvPr id="2" name="Diagramm 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -716,20 +807,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>923925</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>738187</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>19049</xdr:rowOff>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>142874</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="9" name="Diagramm 8"/>
+        <xdr:cNvPr id="6" name="Diagramm 5"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -739,6 +830,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1042987</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>204787</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Diagramm 9"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1034,235 +1155,326 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E1:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
-    <col min="4" max="4" width="24" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="34.85546875" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="24" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>15</v>
       </c>
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>110</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>160</v>
       </c>
-      <c r="D2" s="1">
-        <f>B2/(C2/60)</f>
+      <c r="E2" s="1">
+        <f t="shared" ref="E2:E11" si="0">C2/(D2/60)</f>
         <v>41.25</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>10</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>8</v>
       </c>
+      <c r="H2">
+        <f>D2/C2</f>
+        <v>1.4545454545454546</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>90</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>130</v>
       </c>
-      <c r="D3" s="1">
-        <f>B3/(C3/60)</f>
+      <c r="E3" s="1">
+        <f t="shared" si="0"/>
         <v>41.53846153846154</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>10</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>8</v>
       </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H11" si="1">D3/C3</f>
+        <v>1.4444444444444444</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>50</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>90</v>
       </c>
-      <c r="D4" s="1">
-        <f>B4/(C4/60)</f>
+      <c r="E4" s="1">
+        <f t="shared" si="0"/>
         <v>33.333333333333336</v>
-      </c>
-      <c r="E4">
-        <v>7</v>
       </c>
       <c r="F4">
         <v>7</v>
       </c>
+      <c r="G4">
+        <v>7</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="1"/>
+        <v>1.8</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>40</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>120</v>
       </c>
-      <c r="D5" s="1">
-        <f>B5/(C5/60)</f>
+      <c r="E5" s="1">
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>8</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>3</v>
       </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>5</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>30</v>
       </c>
-      <c r="D6" s="1">
-        <f>B6/(C6/60)</f>
+      <c r="E6" s="1">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>7</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>1</v>
       </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
         <v>8</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>1</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>10</v>
       </c>
-      <c r="D7" s="1">
-        <f>B7/(C7/60)</f>
+      <c r="E7" s="1">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>6</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>1</v>
       </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>4</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>20</v>
       </c>
-      <c r="D8" s="1">
-        <f>B8/(C8/60)</f>
+      <c r="E8" s="1">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>6</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>2</v>
       </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
         <v>10</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>30</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>120</v>
       </c>
-      <c r="D9" s="1">
-        <f>B9/(C9/60)</f>
+      <c r="E9" s="1">
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>5</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>4</v>
       </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
         <v>11</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>20</v>
       </c>
-      <c r="E10">
+      <c r="D10">
+        <v>60</v>
+      </c>
+      <c r="E10" s="1">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="F10">
         <v>2</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>5</v>
       </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
         <v>12</v>
       </c>
-      <c r="B11">
+      <c r="C11">
         <v>70</v>
       </c>
-      <c r="E11">
+      <c r="D11">
+        <v>120</v>
+      </c>
+      <c r="E11" s="1">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="F11">
         <v>1</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>9</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>1.7142857142857142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>